<commit_message>
Adding new data sets
</commit_message>
<xml_diff>
--- a/Contrastchart.xlsx
+++ b/Contrastchart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-32240" yWindow="3980" windowWidth="25600" windowHeight="15020" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="40" windowWidth="25600" windowHeight="15020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>StAug-Buffer-None-None</t>
   </si>
@@ -145,6 +145,21 @@
   </si>
   <si>
     <t>Rhiz(n)::St.Aug=PI</t>
+  </si>
+  <si>
+    <t>Rhiz:soilL-H</t>
+  </si>
+  <si>
+    <t>Rhiz:soilL-N</t>
+  </si>
+  <si>
+    <t>Rhiz:soilN-H</t>
+  </si>
+  <si>
+    <t>Rhiz:Soil-PI=StAug</t>
+  </si>
+  <si>
+    <t>Rhiz:Soil-PI=StAugL</t>
   </si>
 </sst>
 </file>
@@ -184,12 +199,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -219,7 +240,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="109">
+  <cellStyleXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -329,8 +350,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -360,8 +413,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="109">
+  <cellStyles count="141">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -416,6 +478,22 @@
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -470,6 +548,22 @@
     <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -799,10 +893,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:V25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AC10" sqref="AC10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -817,9 +914,11 @@
     <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1">
+    <row r="1" spans="1:22" s="3" customFormat="1">
       <c r="B1" s="5" t="s">
         <v>35</v>
       </c>
@@ -839,8 +938,9 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
-    </row>
-    <row r="2" spans="1:17" s="3" customFormat="1">
+      <c r="U1" s="15"/>
+    </row>
+    <row r="2" spans="1:22" s="3" customFormat="1">
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="4"/>
@@ -862,8 +962,9 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
-    </row>
-    <row r="3" spans="1:17" s="3" customFormat="1">
+      <c r="U2" s="15"/>
+    </row>
+    <row r="3" spans="1:22" s="3" customFormat="1">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
@@ -915,8 +1016,23 @@
       <c r="Q3" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="R3" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="U3" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="V3" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -969,8 +1085,23 @@
       <c r="Q4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="R4" s="14">
+        <v>0</v>
+      </c>
+      <c r="S4" s="14">
+        <v>0</v>
+      </c>
+      <c r="T4" s="14">
+        <v>0</v>
+      </c>
+      <c r="U4" s="17">
+        <v>0</v>
+      </c>
+      <c r="V4" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1022,8 +1153,23 @@
       <c r="Q5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="R5" s="14">
+        <v>0</v>
+      </c>
+      <c r="S5" s="14">
+        <v>-0.5</v>
+      </c>
+      <c r="T5" s="14">
+        <v>-0.5</v>
+      </c>
+      <c r="U5" s="17">
+        <v>0</v>
+      </c>
+      <c r="V5" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1078,8 +1224,23 @@
       <c r="Q6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="R6" s="14">
+        <v>0</v>
+      </c>
+      <c r="S6" s="14">
+        <v>0</v>
+      </c>
+      <c r="T6" s="14">
+        <v>0</v>
+      </c>
+      <c r="U6" s="17">
+        <v>0</v>
+      </c>
+      <c r="V6" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1133,8 +1294,23 @@
       <c r="Q7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="R7" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="S7" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="T7" s="14">
+        <v>0</v>
+      </c>
+      <c r="U7" s="17">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="V7" s="17">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1190,8 +1366,23 @@
       <c r="Q8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="R8" s="14">
+        <v>0</v>
+      </c>
+      <c r="S8" s="14">
+        <v>0</v>
+      </c>
+      <c r="T8" s="14">
+        <v>0</v>
+      </c>
+      <c r="U8" s="17">
+        <v>0</v>
+      </c>
+      <c r="V8" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1246,8 +1437,23 @@
       <c r="Q9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="R9" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="S9" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="T9" s="14">
+        <v>0</v>
+      </c>
+      <c r="U9" s="17">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="V9" s="17">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1302,8 +1508,23 @@
       <c r="Q10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="R10" s="14">
+        <v>-0.5</v>
+      </c>
+      <c r="S10" s="14">
+        <v>0</v>
+      </c>
+      <c r="T10" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="U10" s="17">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="V10" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1355,8 +1576,23 @@
       <c r="Q11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="R11" s="14">
+        <v>0</v>
+      </c>
+      <c r="S11" s="14">
+        <v>0</v>
+      </c>
+      <c r="T11" s="14">
+        <v>0</v>
+      </c>
+      <c r="U11" s="17">
+        <v>0</v>
+      </c>
+      <c r="V11" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1408,8 +1644,23 @@
       <c r="Q12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="R12" s="14">
+        <v>0</v>
+      </c>
+      <c r="S12" s="14">
+        <v>-0.5</v>
+      </c>
+      <c r="T12" s="14">
+        <v>-0.5</v>
+      </c>
+      <c r="U12" s="17">
+        <v>0</v>
+      </c>
+      <c r="V12" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1464,8 +1715,23 @@
       <c r="Q13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="R13" s="14">
+        <v>0</v>
+      </c>
+      <c r="S13" s="14">
+        <v>0</v>
+      </c>
+      <c r="T13" s="14">
+        <v>0</v>
+      </c>
+      <c r="U13" s="17">
+        <v>0</v>
+      </c>
+      <c r="V13" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1520,8 +1786,23 @@
       <c r="Q14">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="R14" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="S14" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="T14" s="14">
+        <v>0</v>
+      </c>
+      <c r="U14" s="17">
+        <v>-0.33333333333333331</v>
+      </c>
+      <c r="V14" s="17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -1576,8 +1857,23 @@
       <c r="Q15">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="R15" s="14">
+        <v>-0.5</v>
+      </c>
+      <c r="S15" s="14">
+        <v>0</v>
+      </c>
+      <c r="T15" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="U15" s="17">
+        <v>-0.33333333333333331</v>
+      </c>
+      <c r="V15" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -1630,8 +1926,23 @@
       <c r="Q16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="R16" s="14">
+        <v>0</v>
+      </c>
+      <c r="S16" s="14">
+        <v>0</v>
+      </c>
+      <c r="T16" s="14">
+        <v>0</v>
+      </c>
+      <c r="U16" s="17">
+        <v>0</v>
+      </c>
+      <c r="V16" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -1684,33 +1995,48 @@
       <c r="Q17">
         <v>-1</v>
       </c>
-    </row>
-    <row r="20" spans="1:17">
+      <c r="R17" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="S17" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="T17" s="14">
+        <v>0</v>
+      </c>
+      <c r="U17" s="17">
+        <v>-0.33333333333333331</v>
+      </c>
+      <c r="V17" s="17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22">
       <c r="A20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:22">
       <c r="A21" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:22">
       <c r="A22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:22">
       <c r="A23" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:22">
       <c r="A24" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:22">
       <c r="A25" t="s">
         <v>33</v>
       </c>

</xml_diff>